<commit_message>
feat(labs): :sparkles: Saving work from excel sheet from labs
</commit_message>
<xml_diff>
--- a/Labs/Lab 2/Lab 2.xlsx
+++ b/Labs/Lab 2/Lab 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Labs\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D8ED56-7FD4-431E-AD14-70540C67AA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAFE3F9-1D9D-4FAD-BD57-317A6D359D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>R</t>
   </si>
   <si>
-    <t>V</t>
+    <t>V(sim)</t>
   </si>
   <si>
-    <t>P</t>
+    <t>P(sim)</t>
+  </si>
+  <si>
+    <t>P(theo)</t>
+  </si>
+  <si>
+    <t>V(theo)</t>
   </si>
 </sst>
 </file>
@@ -211,7 +217,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>V</c:v>
+                  <c:v>V(theo)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -304,7 +310,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P</c:v>
+                  <c:v>P(theo)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -385,6 +391,192 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DB6E-46A7-A0D8-9A270593C641}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V(sim)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-457A-4D29-85F1-B9C03812FCF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P(sim)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>42.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-457A-4D29-85F1-B9C03812FCF0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -713,7 +905,761 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>Power/Voltage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NZ" baseline="0"/>
+              <a:t> vs Resistance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-NZ"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V(theo)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$30:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$30:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3D01-4426-9A18-680B3DC97163}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P(theo)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$30:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$30:$F$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3D01-4426-9A18-680B3DC97163}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V(sim)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$30:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$30:$G$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3D01-4426-9A18-680B3DC97163}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P(sim)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$30:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$30:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8699999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3D01-4426-9A18-680B3DC97163}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="645987375"/>
+        <c:axId val="645986895"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="645987375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Resistance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> (Ohms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="645986895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="645986895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Volgage (V) / Power (W)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="645987375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1269,20 +2215,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>10885</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63894</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>169049</xdr:rowOff>
+      <xdr:rowOff>23275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>534041</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>42454</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>587050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>82211</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1302,6 +2764,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>18709</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>26895</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>170329</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50BF9D62-8C85-F938-3FEF-673BD7028B91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1627,26 +3125,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786A0C80-D68D-4C69-80F8-C85B7F5926AC}">
-  <dimension ref="C5:E12"/>
+  <dimension ref="C5:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -1656,8 +3160,14 @@
       <c r="E6" s="1">
         <v>50</v>
       </c>
+      <c r="F6" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="G6" s="1">
+        <v>42.78</v>
+      </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>4</v>
       </c>
@@ -1667,8 +3177,14 @@
       <c r="E7" s="1">
         <v>25</v>
       </c>
+      <c r="F7" s="1">
+        <v>9.61</v>
+      </c>
+      <c r="G7" s="1">
+        <v>23.09</v>
+      </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <v>6</v>
       </c>
@@ -1678,8 +3194,14 @@
       <c r="E8" s="1">
         <v>16.670000000000002</v>
       </c>
+      <c r="F8" s="1">
+        <v>9.74</v>
+      </c>
+      <c r="G8" s="1">
+        <v>15.8</v>
+      </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <v>8</v>
       </c>
@@ -1689,8 +3211,14 @@
       <c r="E9" s="1">
         <v>12.5</v>
       </c>
+      <c r="F9" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G9" s="1">
+        <v>12</v>
+      </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <v>10</v>
       </c>
@@ -1700,15 +3228,123 @@
       <c r="E10" s="1">
         <v>10</v>
       </c>
+      <c r="F10" s="1">
+        <v>9.84</v>
+      </c>
+      <c r="G10" s="1">
+        <v>9.68</v>
+      </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
+    </row>
+    <row r="29" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1">
+        <v>50</v>
+      </c>
+      <c r="G30" s="1">
+        <v>3.18</v>
+      </c>
+      <c r="H30" s="1">
+        <v>5.07</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D31" s="1">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1">
+        <v>25</v>
+      </c>
+      <c r="G31" s="1">
+        <v>6.37</v>
+      </c>
+      <c r="H31" s="1">
+        <v>10.130000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D32" s="1">
+        <v>6</v>
+      </c>
+      <c r="E32" s="1">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="G32" s="1">
+        <v>9.33</v>
+      </c>
+      <c r="H32" s="1">
+        <v>14.51</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D33" s="1">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="G33" s="1">
+        <v>9.77</v>
+      </c>
+      <c r="H33" s="1">
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D34" s="1">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1">
+        <v>10</v>
+      </c>
+      <c r="F34" s="1">
+        <v>10</v>
+      </c>
+      <c r="G34" s="1">
+        <v>9.93</v>
+      </c>
+      <c r="H34" s="1">
+        <v>9.8699999999999992</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel for lab 2
</commit_message>
<xml_diff>
--- a/Labs/Lab 2/Lab 2.xlsx
+++ b/Labs/Lab 2/Lab 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Labs\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAFE3F9-1D9D-4FAD-BD57-317A6D359D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DD51B5-DC7D-4395-9452-223CB12F4346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1042,13 +1042,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
@@ -1123,13 +1123,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>5.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>10.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.670000000000002</c:v>
+                  <c:v>15.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12.5</c:v>
@@ -1288,7 +1288,7 @@
                   <c:v>5.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.130000000000001</c:v>
+                  <c:v>10.26</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>14.51</c:v>
@@ -3127,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786A0C80-D68D-4C69-80F8-C85B7F5926AC}">
   <dimension ref="C5:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3266,10 +3266,10 @@
         <v>2</v>
       </c>
       <c r="E30" s="1">
-        <v>10</v>
+        <v>3.2</v>
       </c>
       <c r="F30" s="1">
-        <v>50</v>
+        <v>5.12</v>
       </c>
       <c r="G30" s="1">
         <v>3.18</v>
@@ -3283,16 +3283,16 @@
         <v>4</v>
       </c>
       <c r="E31" s="1">
-        <v>10</v>
+        <v>6.5</v>
       </c>
       <c r="F31" s="1">
-        <v>25</v>
+        <v>10.24</v>
       </c>
       <c r="G31" s="1">
         <v>6.37</v>
       </c>
       <c r="H31" s="1">
-        <v>10.130000000000001</v>
+        <v>10.26</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.3">
@@ -3300,10 +3300,10 @@
         <v>6</v>
       </c>
       <c r="E32" s="1">
-        <v>10</v>
+        <v>9.6</v>
       </c>
       <c r="F32" s="1">
-        <v>16.670000000000002</v>
+        <v>15.46</v>
       </c>
       <c r="G32" s="1">
         <v>9.33</v>

</xml_diff>

<commit_message>
feat(labs): :sparkles: Updated excels sheets
</commit_message>
<xml_diff>
--- a/Labs/Lab 2/Lab 2.xlsx
+++ b/Labs/Lab 2/Lab 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Labs\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DD51B5-DC7D-4395-9452-223CB12F4346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B0A012-AFB0-4846-BF17-DAB731650C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12696" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>R</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>V(theo)</t>
+  </si>
+  <si>
+    <t>I_L</t>
   </si>
 </sst>
 </file>
@@ -3125,10 +3128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786A0C80-D68D-4C69-80F8-C85B7F5926AC}">
-  <dimension ref="C5:H34"/>
+  <dimension ref="C5:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3346,6 +3349,96 @@
         <v>9.8699999999999992</v>
       </c>
     </row>
+    <row r="61" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D62" s="1">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1">
+        <v>5.3659999999999997</v>
+      </c>
+      <c r="F62" s="1">
+        <v>14.39</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D63" s="1">
+        <v>4</v>
+      </c>
+      <c r="E63" s="1">
+        <v>7.5890000000000004</v>
+      </c>
+      <c r="F63" s="1">
+        <v>14.39</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D64" s="1">
+        <v>6</v>
+      </c>
+      <c r="E64" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F64" s="1">
+        <v>14.39</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D65" s="1">
+        <v>8</v>
+      </c>
+      <c r="E65" s="1">
+        <v>10</v>
+      </c>
+      <c r="F65" s="1">
+        <v>13.42</v>
+      </c>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D66" s="1">
+        <v>10</v>
+      </c>
+      <c r="E66" s="1">
+        <v>10</v>
+      </c>
+      <c r="F66" s="1">
+        <v>12</v>
+      </c>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
feat(labs): :sparkles: Added excel files for lab 2
</commit_message>
<xml_diff>
--- a/Labs/Lab 2/Lab 2.xlsx
+++ b/Labs/Lab 2/Lab 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Labs\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B0A012-AFB0-4846-BF17-DAB731650C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46F88F6-0D32-4A39-BE0F-B60D6AC7ABB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12696" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3130,8 +3130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786A0C80-D68D-4C69-80F8-C85B7F5926AC}">
   <dimension ref="C5:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3379,9 +3379,15 @@
       <c r="F62" s="1">
         <v>14.39</v>
       </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
+      <c r="G62" s="1">
+        <v>2.02</v>
+      </c>
+      <c r="H62" s="1">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="I62" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D63" s="1">
@@ -3393,9 +3399,15 @@
       <c r="F63" s="1">
         <v>14.39</v>
       </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
+      <c r="G63" s="1">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="H63" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D64" s="1">
@@ -3407,9 +3419,15 @@
       <c r="F64" s="1">
         <v>14.39</v>
       </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
+      <c r="G64" s="1">
+        <v>6.02</v>
+      </c>
+      <c r="H64" s="1">
+        <v>6.04</v>
+      </c>
+      <c r="I64" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D65" s="1">
@@ -3419,11 +3437,17 @@
         <v>10</v>
       </c>
       <c r="F65" s="1">
-        <v>13.42</v>
-      </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="G65" s="1">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="H65" s="1">
+        <v>8.01</v>
+      </c>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D66" s="1">
@@ -3433,11 +3457,17 @@
         <v>10</v>
       </c>
       <c r="F66" s="1">
-        <v>12</v>
-      </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G66" s="1">
+        <v>10</v>
+      </c>
+      <c r="H66" s="1">
+        <v>10</v>
+      </c>
+      <c r="I66" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat(labs): :sparkles: Finished lab2, added matlab simulation files for task 4 and final excel spreadsheet
</commit_message>
<xml_diff>
--- a/Labs/Lab 2/Lab 2.xlsx
+++ b/Labs/Lab 2/Lab 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Labs\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46F88F6-0D32-4A39-BE0F-B60D6AC7ABB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF4BBCE-C344-4D7D-A326-B97B126E1F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C8D5DF51-7E4A-49B5-BBD2-E36A7104CD81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>R</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>V(theo)</t>
-  </si>
-  <si>
-    <t>I_L</t>
   </si>
 </sst>
 </file>
@@ -78,12 +75,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -107,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,6 +118,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1622,6 +1626,777 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Power/Voltage vs Resistance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V(theo)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$62:$D$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$62:$E$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.3659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F138-44E2-B6AC-A1F1CDDB6169}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P(theo)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$62:$D$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$62:$F$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>14.39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F138-44E2-B6AC-A1F1CDDB6169}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V(sim)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$62:$D$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$62:$G$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F138-44E2-B6AC-A1F1CDDB6169}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P(sim)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$62:$D$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$62:$H$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9600000000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F138-44E2-B6AC-A1F1CDDB6169}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$62:$D$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$62:$I$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F138-44E2-B6AC-A1F1CDDB6169}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1066814543"/>
+        <c:axId val="1066794383"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1066814543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Resistance (Ohms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1066794383"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1066794383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Voltage (V) / Power (W)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1066814543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1702,6 +2477,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2219,6 +3034,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2803,6 +4134,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>37171</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>55756</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>573629</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>1749</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB80EA7C-BA6C-2DD3-8A31-DDD08330058B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3130,8 +4497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786A0C80-D68D-4C69-80F8-C85B7F5926AC}">
   <dimension ref="C5:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="62" zoomScaleNormal="36" workbookViewId="0">
+      <selection activeCell="X53" sqref="X53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3349,7 +4716,7 @@
         <v>9.8699999999999992</v>
       </c>
     </row>
-    <row r="61" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D61" s="2" t="s">
         <v>0</v>
       </c>
@@ -3365,11 +4732,9 @@
       <c r="H61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D62" s="1">
         <v>2</v>
       </c>
@@ -3380,16 +4745,15 @@
         <v>14.39</v>
       </c>
       <c r="G62" s="1">
+        <v>5</v>
+      </c>
+      <c r="H62" s="1">
         <v>2.02</v>
       </c>
-      <c r="H62" s="1">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="I62" s="1">
-        <v>1</v>
-      </c>
+      <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C63" s="3"/>
       <c r="D63" s="1">
         <v>4</v>
       </c>
@@ -3405,11 +4769,10 @@
       <c r="H63" s="1">
         <v>4.05</v>
       </c>
-      <c r="I63" s="1">
-        <v>1</v>
-      </c>
+      <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C64" s="3"/>
       <c r="D64" s="1">
         <v>6</v>
       </c>
@@ -3425,9 +4788,7 @@
       <c r="H64" s="1">
         <v>6.04</v>
       </c>
-      <c r="I64" s="1">
-        <v>1</v>
-      </c>
+      <c r="I64" s="1"/>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D65" s="1">
@@ -3440,14 +4801,12 @@
         <v>12.5</v>
       </c>
       <c r="G65" s="1">
-        <v>8.0299999999999994</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="H65" s="1">
-        <v>8.01</v>
-      </c>
-      <c r="I65" s="1">
-        <v>1</v>
-      </c>
+        <v>12.5</v>
+      </c>
+      <c r="I65" s="1"/>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D66" s="1">
@@ -3463,11 +4822,9 @@
         <v>10</v>
       </c>
       <c r="H66" s="1">
-        <v>10</v>
-      </c>
-      <c r="I66" s="1">
-        <v>1</v>
-      </c>
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="I66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>